<commit_message>
Downstream Task: Polartity Detection Analysis
</commit_message>
<xml_diff>
--- a/data/data_file1.xlsx
+++ b/data/data_file1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>antonym_1</t>
   </si>
@@ -106,19 +106,33 @@
     <t>low speed</t>
   </si>
   <si>
-    <t>good</t>
-  </si>
-  <si>
-    <t>bad</t>
+    <t>good_0</t>
+  </si>
+  <si>
+    <t>bad_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eating healthy food is good for you.
+</t>
+  </si>
+  <si>
+    <t>Smoking is bad for your health.</t>
+  </si>
+  <si>
+    <t>positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">negative
+</t>
+  </si>
+  <si>
+    <t>good_1</t>
+  </si>
+  <si>
+    <t>bad_1</t>
   </si>
   <si>
     <t>Eating healthy food is good for you.</t>
-  </si>
-  <si>
-    <t>Smoking is bad for your health.</t>
-  </si>
-  <si>
-    <t>positive</t>
   </si>
   <si>
     <t>negative</t>
@@ -468,7 +482,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -602,6 +616,26 @@
         <v>35</v>
       </c>
     </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+      <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>